<commit_message>
Listo para conectarlo a MongoDB. Falta envios masivos
</commit_message>
<xml_diff>
--- a/chats/clientes-saludar.xlsx
+++ b/chats/clientes-saludar.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D7B357-417C-4692-8A81-428079BF1585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="28800" windowHeight="12465"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,12 +14,8 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
@@ -333,19 +330,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>51970749820</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>51946361875</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>

</xml_diff>